<commit_message>
commit message user module03
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Team05-API Squad Test Data.xlsx
+++ b/src/test/resources/TestData/Team05-API Squad Test Data.xlsx
@@ -5,29 +5,25 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayau\OneDrive\Desktop\GIT-TEAM5-REST ASSURED-JAN 2026\Team 5 Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rajav\git\Team05_APISquad\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7ED3BF9-EEB5-46FD-B501-3C27E8D6994D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53ED362-EC13-4E02-8CFD-06CFA35B4247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="600" windowWidth="29040" windowHeight="15000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Program" sheetId="2" r:id="rId2"/>
     <sheet name="Batch" sheetId="3" r:id="rId3"/>
+    <sheet name="User" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="V7gfgs95oMe8R0X1XyBm5VQ3wOPA245uiiS1n805UL0="/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="221">
   <si>
     <t>ScenarioName</t>
   </si>
@@ -583,16 +579,131 @@
   <si>
     <t>Get Batch Details by Batch Id</t>
   </si>
+  <si>
+    <t>Create_Valid_User</t>
+  </si>
+  <si>
+    <t>/users/roleStatus</t>
+  </si>
+  <si>
+    <t>userComments</t>
+  </si>
+  <si>
+    <t>userEduPg</t>
+  </si>
+  <si>
+    <t>userEduUg</t>
+  </si>
+  <si>
+    <t>userFirstName</t>
+  </si>
+  <si>
+    <t>userLastName</t>
+  </si>
+  <si>
+    <t>userLinkedinUrl</t>
+  </si>
+  <si>
+    <t>userLocation</t>
+  </si>
+  <si>
+    <t>userMiddleName</t>
+  </si>
+  <si>
+    <t>userPhoneNumber</t>
+  </si>
+  <si>
+    <t>userRoleMaps</t>
+  </si>
+  <si>
+    <t>userTimeZone</t>
+  </si>
+  <si>
+    <t>userVisaStatus</t>
+  </si>
+  <si>
+    <t>userLogin</t>
+  </si>
+  <si>
+    <t>userId</t>
+  </si>
+  <si>
+    <t>roleId</t>
+  </si>
+  <si>
+    <t>userRoleList</t>
+  </si>
+  <si>
+    <t>userRoleProgramBatches</t>
+  </si>
+  <si>
+    <t>loginStatus</t>
+  </si>
+  <si>
+    <t>roleIds</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>userLoginEmail</t>
+  </si>
+  <si>
+    <t>Create a new User</t>
+  </si>
+  <si>
+    <t>MCA</t>
+  </si>
+  <si>
+    <t>BSC</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>CST</t>
+  </si>
+  <si>
+    <t>H4</t>
+  </si>
+  <si>
+    <t>+91 9675343333</t>
+  </si>
+  <si>
+    <t>Prashanthiyz</t>
+  </si>
+  <si>
+    <t>Rakeshxzx</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/Prashanthi1/</t>
+  </si>
+  <si>
+    <t>[{"roleId":"R01","userRoleStatus":"Active"}</t>
+  </si>
+  <si>
+    <t>{"userLoginEmail":"Prasha3w5hieiy1wp@gmail.com","loginStatus":"Active","status":"Active"}'</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -685,8 +796,37 @@
       <name val="Aptos"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -721,6 +861,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFD966"/>
         <bgColor rgb="FFFFD966"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF60CBF3"/>
+        <bgColor rgb="FF60CBF3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCAEDFB"/>
+        <bgColor rgb="FFCAEDFB"/>
       </patternFill>
     </fill>
   </fills>
@@ -785,107 +937,126 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -31963,8 +32134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AB1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -34222,6 +34393,199 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4288ABC0-DE51-4F1D-BF0D-EE92A041B4A9}">
+  <dimension ref="A1:AF3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="5" max="5" width="32.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" customWidth="1"/>
+    <col min="13" max="13" width="19.7109375" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" customWidth="1"/>
+    <col min="15" max="15" width="18" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" customWidth="1"/>
+    <col min="17" max="17" width="67.140625" customWidth="1"/>
+    <col min="21" max="21" width="64" customWidth="1"/>
+    <col min="24" max="24" width="87.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" ht="14.25" customHeight="1">
+      <c r="A1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="H1" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="I1" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="J1" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="49" t="s">
+        <v>187</v>
+      </c>
+      <c r="M1" s="49" t="s">
+        <v>188</v>
+      </c>
+      <c r="N1" s="49" t="s">
+        <v>189</v>
+      </c>
+      <c r="O1" s="49" t="s">
+        <v>190</v>
+      </c>
+      <c r="P1" s="49" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q1" s="49" t="s">
+        <v>192</v>
+      </c>
+      <c r="R1" s="49" t="s">
+        <v>193</v>
+      </c>
+      <c r="S1" s="49" t="s">
+        <v>194</v>
+      </c>
+      <c r="T1" s="49" t="s">
+        <v>195</v>
+      </c>
+      <c r="U1" s="49" t="s">
+        <v>196</v>
+      </c>
+      <c r="V1" s="49" t="s">
+        <v>197</v>
+      </c>
+      <c r="W1" s="49" t="s">
+        <v>198</v>
+      </c>
+      <c r="X1" s="49" t="s">
+        <v>199</v>
+      </c>
+      <c r="Y1" s="49" t="s">
+        <v>200</v>
+      </c>
+      <c r="Z1" s="49" t="s">
+        <v>201</v>
+      </c>
+      <c r="AA1" s="49" t="s">
+        <v>202</v>
+      </c>
+      <c r="AB1" s="49" t="s">
+        <v>203</v>
+      </c>
+      <c r="AC1" s="49" t="s">
+        <v>204</v>
+      </c>
+      <c r="AD1" s="49" t="s">
+        <v>205</v>
+      </c>
+      <c r="AE1" s="49" t="s">
+        <v>206</v>
+      </c>
+      <c r="AF1" s="49" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32">
+      <c r="A2" s="47" t="s">
+        <v>185</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>186</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="50" t="s">
+        <v>208</v>
+      </c>
+      <c r="M2" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="N2" s="50" t="s">
+        <v>210</v>
+      </c>
+      <c r="O2" s="50" t="s">
+        <v>216</v>
+      </c>
+      <c r="P2" s="50" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q2" s="53" t="s">
+        <v>218</v>
+      </c>
+      <c r="R2" s="50" t="s">
+        <v>211</v>
+      </c>
+      <c r="S2" s="50" t="s">
+        <v>212</v>
+      </c>
+      <c r="T2" s="51" t="s">
+        <v>215</v>
+      </c>
+      <c r="U2" s="52" t="s">
+        <v>219</v>
+      </c>
+      <c r="V2" s="50" t="s">
+        <v>213</v>
+      </c>
+      <c r="W2" s="50" t="s">
+        <v>214</v>
+      </c>
+      <c r="X2" s="51" t="s">
+        <v>220</v>
+      </c>
+      <c r="Y2" s="50"/>
+      <c r="Z2" s="50"/>
+    </row>
+    <row r="3" spans="1:32">
+      <c r="A3" s="47"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="Q2" r:id="rId1" xr:uid="{E3FE39B1-0B35-42D0-ACBB-B7E8C451EFCD}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{d9290083-bd2f-48a2-8ac5-09a524b17d15}" enabled="1" method="Privileged" siteId="{b9fec68c-c92d-461e-9a97-3d03a0f18b82}" contentBits="1" removed="0"/>

</xml_diff>

<commit_message>
Resolved merge conflicts - kept team Excel file and local log
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Team05-API Squad Test Data.xlsx
+++ b/src/test/resources/TestData/Team05-API Squad Test Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rajav\git\Team05_APISquad\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayau\OneDrive\Desktop\GIT-TEAM5-REST ASSURED-JAN 2026\Team05_APISquad\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E92AAD-ADDA-49E0-B145-7ACB4DCC0402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C7CFAE-8EFC-4F5C-9DD1-451FD5C85DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30585" yWindow="2370" windowWidth="18000" windowHeight="9270" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="600" windowWidth="29040" windowHeight="15000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="236">
   <si>
     <t>ScenarioName</t>
   </si>
@@ -424,9 +424,6 @@
     <t>programName</t>
   </si>
   <si>
-    <t>Existing batch Number</t>
-  </si>
-  <si>
     <t>batches</t>
   </si>
   <si>
@@ -673,46 +670,78 @@
     <t>+91 9675343333</t>
   </si>
   <si>
+    <t>Prashanthiyz</t>
+  </si>
+  <si>
+    <t>Rakeshxzx</t>
+  </si>
+  <si>
     <t>https://www.linkedin.com/in/Prashanthi1/</t>
   </si>
   <si>
-    <t>GetallusersValidEndpoint</t>
+    <t>[{"roleId":"R01","userRoleStatus":"Active"}</t>
   </si>
   <si>
-    <t>/users</t>
+    <t>{"userLoginEmail":"Prasha3w5hieiy1wp@gmail.com","loginStatus":"Active","status":"Active"}'</t>
   </si>
   <si>
-    <t>{"userLoginEmail":"...","loginStatus":"Active","status":"Active"}</t>
+    <t>Existing batch Name</t>
   </si>
   <si>
-    <t>R01</t>
+    <t>APISquad001</t>
   </si>
   <si>
-    <t>Prashanthiyzu</t>
+    <t>Team5 Batch Java</t>
   </si>
   <si>
-    <t>Rakeshxzxrahavi</t>
+    <t>UnitTesting</t>
   </si>
   <si>
-    <t>[{"roleId": "R01", "userRoleStatus": "Active"}]</t>
+    <t>InvalidBatchNameFormat</t>
+  </si>
+  <si>
+    <t>123APISquad</t>
+  </si>
+  <si>
+    <t>MissingBatchName</t>
+  </si>
+  <si>
+    <t>""</t>
+  </si>
+  <si>
+    <t>SequenceMoreThan99</t>
+  </si>
+  <si>
+    <t>APISquad7759</t>
+  </si>
+  <si>
+    <t>NegativeClasses</t>
+  </si>
+  <si>
+    <t>InvalidStatus</t>
+  </si>
+  <si>
+    <t>INVALID</t>
+  </si>
+  <si>
+    <t>APISquad101</t>
+  </si>
+  <si>
+    <t>batchDescription</t>
+  </si>
+  <si>
+    <t>batchNoOfClasses</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -830,30 +859,39 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -900,6 +938,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFCAEDFB"/>
         <bgColor rgb="FFCAEDFB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -966,123 +1016,127 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -29427,8 +29481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB1012"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:J2"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -29440,7 +29494,7 @@
     <col min="6" max="6" width="25" customWidth="1"/>
     <col min="7" max="8" width="25.42578125" customWidth="1"/>
     <col min="9" max="9" width="19.85546875" customWidth="1"/>
-    <col min="10" max="10" width="114.42578125" customWidth="1"/>
+    <col min="10" max="10" width="36.85546875" customWidth="1"/>
     <col min="11" max="28" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -32161,29 +32215,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AB1002"/>
+  <dimension ref="A1:AD1007"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="42.5703125" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" customWidth="1"/>
-    <col min="10" max="10" width="7.42578125" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" customWidth="1"/>
-    <col min="12" max="26" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="5" max="7" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" customWidth="1"/>
+    <col min="12" max="12" width="15" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" customWidth="1"/>
+    <col min="14" max="28" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="14.25" customHeight="1">
+    <row r="1" spans="1:30" ht="14.25" customHeight="1">
       <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
@@ -32200,40 +32254,46 @@
         <v>128</v>
       </c>
       <c r="F1" s="32" t="s">
+        <v>234</v>
+      </c>
+      <c r="G1" s="32" t="s">
+        <v>235</v>
+      </c>
+      <c r="H1" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="I1" s="32" t="s">
         <v>130</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="J1" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="K1" s="32" t="s">
         <v>132</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="L1" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="M1" s="32" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="14.25" customHeight="1">
+    <row r="2" spans="1:30" ht="14.25" customHeight="1">
       <c r="A2" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" s="34"/>
       <c r="C2" s="34"/>
       <c r="D2" s="34"/>
       <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
       <c r="H2" s="34"/>
       <c r="I2" s="34"/>
       <c r="J2" s="34"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="35"/>
       <c r="N2" s="11"/>
       <c r="O2" s="11"/>
       <c r="P2" s="11"/>
@@ -32249,13 +32309,15 @@
       <c r="Z2" s="11"/>
       <c r="AA2" s="11"/>
       <c r="AB2" s="11"/>
-    </row>
-    <row r="3" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A3" s="36" t="s">
+      <c r="AC2" s="11"/>
+      <c r="AD2" s="11"/>
+    </row>
+    <row r="3" spans="1:30" s="59" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A3" s="54" t="s">
+        <v>220</v>
+      </c>
+      <c r="B3" s="54" t="s">
         <v>133</v>
-      </c>
-      <c r="B3" s="36" t="s">
-        <v>134</v>
       </c>
       <c r="C3" s="37" t="s">
         <v>10</v>
@@ -32264,481 +32326,765 @@
         <v>11</v>
       </c>
       <c r="E3" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="F3" s="55" t="s">
+        <v>222</v>
+      </c>
+      <c r="G3" s="55">
+        <v>34</v>
+      </c>
+      <c r="H3" s="54" t="s">
         <v>135</v>
       </c>
-      <c r="F3" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="G3" s="37">
-        <v>16331</v>
-      </c>
-      <c r="H3" s="37">
+      <c r="I3" s="56">
+        <v>39</v>
+      </c>
+      <c r="J3" s="37">
         <v>10101</v>
       </c>
-      <c r="I3" s="37" t="s">
+      <c r="K3" s="56" t="s">
+        <v>223</v>
+      </c>
+      <c r="L3" s="37">
+        <v>400</v>
+      </c>
+      <c r="M3" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="N3" s="58"/>
+      <c r="O3" s="58"/>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="58"/>
+      <c r="R3" s="58"/>
+      <c r="S3" s="58"/>
+      <c r="T3" s="58"/>
+      <c r="U3" s="58"/>
+      <c r="V3" s="58"/>
+      <c r="W3" s="58"/>
+      <c r="X3" s="58"/>
+      <c r="Y3" s="58"/>
+      <c r="Z3" s="58"/>
+      <c r="AA3" s="58"/>
+      <c r="AB3" s="58"/>
+      <c r="AC3" s="58"/>
+      <c r="AD3" s="58"/>
+    </row>
+    <row r="4" spans="1:30" s="59" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A4" s="54" t="s">
         <v>137</v>
       </c>
-      <c r="J3" s="37">
-        <v>400</v>
-      </c>
-      <c r="K3" s="36" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A4" s="36" t="s">
-        <v>138</v>
-      </c>
-      <c r="B4" s="36" t="s">
-        <v>134</v>
+      <c r="B4" s="54" t="s">
+        <v>133</v>
       </c>
       <c r="C4" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="36" t="s">
+      <c r="D4" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="55" t="s">
+        <v>221</v>
+      </c>
+      <c r="F4" s="55" t="s">
+        <v>222</v>
+      </c>
+      <c r="G4" s="55">
+        <v>23</v>
+      </c>
+      <c r="H4" s="54" t="s">
         <v>135</v>
       </c>
-      <c r="F4" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="G4" s="37">
-        <v>16331</v>
-      </c>
-      <c r="H4" s="37">
+      <c r="I4" s="56">
+        <v>39</v>
+      </c>
+      <c r="J4" s="37">
         <v>10101</v>
       </c>
-      <c r="I4" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="J4" s="37">
+      <c r="K4" s="56" t="s">
+        <v>223</v>
+      </c>
+      <c r="L4" s="37">
         <v>400</v>
       </c>
-      <c r="K4" s="36" t="s">
+      <c r="M4" s="54" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="5" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A5" s="36" t="s">
-        <v>139</v>
-      </c>
-      <c r="B5" s="36" t="s">
-        <v>134</v>
+      <c r="N4" s="58"/>
+      <c r="O4" s="58"/>
+      <c r="P4" s="58"/>
+      <c r="Q4" s="58"/>
+      <c r="R4" s="58"/>
+      <c r="S4" s="58"/>
+      <c r="T4" s="58"/>
+      <c r="U4" s="58"/>
+      <c r="V4" s="58"/>
+      <c r="W4" s="58"/>
+      <c r="X4" s="58"/>
+      <c r="Y4" s="58"/>
+      <c r="Z4" s="58"/>
+      <c r="AA4" s="58"/>
+      <c r="AB4" s="58"/>
+      <c r="AC4" s="58"/>
+      <c r="AD4" s="58"/>
+    </row>
+    <row r="5" spans="1:30" s="59" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A5" s="54" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" s="54" t="s">
+        <v>133</v>
       </c>
       <c r="C5" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="55" t="s">
+        <v>221</v>
+      </c>
+      <c r="F5" s="55" t="s">
+        <v>222</v>
+      </c>
+      <c r="G5" s="55">
+        <v>35</v>
+      </c>
+      <c r="H5" s="54" t="s">
         <v>135</v>
       </c>
-      <c r="F5" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="G5" s="37">
-        <v>16331</v>
-      </c>
-      <c r="H5" s="37">
+      <c r="I5" s="56">
+        <v>39</v>
+      </c>
+      <c r="J5" s="37">
         <v>10101</v>
       </c>
-      <c r="I5" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="J5" s="37">
+      <c r="K5" s="56" t="s">
+        <v>223</v>
+      </c>
+      <c r="L5" s="37">
         <v>201</v>
       </c>
-      <c r="K5" s="36" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A6" s="36" t="s">
-        <v>141</v>
-      </c>
-      <c r="B6" s="36" t="s">
-        <v>142</v>
+      <c r="M5" s="54" t="s">
+        <v>139</v>
+      </c>
+      <c r="N5" s="58"/>
+      <c r="O5" s="58"/>
+      <c r="P5" s="58"/>
+      <c r="Q5" s="58"/>
+      <c r="R5" s="58"/>
+      <c r="S5" s="58"/>
+      <c r="T5" s="58"/>
+      <c r="U5" s="58"/>
+      <c r="V5" s="58"/>
+      <c r="W5" s="58"/>
+      <c r="X5" s="58"/>
+      <c r="Y5" s="58"/>
+      <c r="Z5" s="58"/>
+      <c r="AA5" s="58"/>
+      <c r="AB5" s="58"/>
+      <c r="AC5" s="58"/>
+      <c r="AD5" s="58"/>
+    </row>
+    <row r="6" spans="1:30" s="59" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A6" s="54" t="s">
+        <v>224</v>
+      </c>
+      <c r="B6" s="54" t="s">
+        <v>133</v>
       </c>
       <c r="C6" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="55" t="s">
+        <v>225</v>
+      </c>
+      <c r="F6" s="55" t="s">
+        <v>222</v>
+      </c>
+      <c r="G6" s="55">
+        <v>23</v>
+      </c>
+      <c r="H6" s="54" t="s">
         <v>135</v>
       </c>
-      <c r="F6" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="G6" s="37">
-        <v>16331</v>
-      </c>
-      <c r="H6" s="37">
+      <c r="I6" s="56">
+        <v>39</v>
+      </c>
+      <c r="J6" s="37">
         <v>10101</v>
       </c>
-      <c r="I6" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="J6" s="37">
+      <c r="K6" s="56" t="s">
+        <v>223</v>
+      </c>
+      <c r="L6" s="37">
+        <v>400</v>
+      </c>
+      <c r="M6" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="N6" s="58"/>
+      <c r="O6" s="58"/>
+      <c r="P6" s="58"/>
+      <c r="Q6" s="58"/>
+      <c r="R6" s="58"/>
+      <c r="S6" s="58"/>
+      <c r="T6" s="58"/>
+      <c r="U6" s="58"/>
+      <c r="V6" s="58"/>
+      <c r="W6" s="58"/>
+      <c r="X6" s="58"/>
+      <c r="Y6" s="58"/>
+      <c r="Z6" s="58"/>
+      <c r="AA6" s="58"/>
+      <c r="AB6" s="58"/>
+      <c r="AC6" s="58"/>
+      <c r="AD6" s="58"/>
+    </row>
+    <row r="7" spans="1:30" s="59" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A7" s="54" t="s">
+        <v>226</v>
+      </c>
+      <c r="B7" s="54" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="55" t="s">
+        <v>227</v>
+      </c>
+      <c r="F7" s="55" t="s">
+        <v>222</v>
+      </c>
+      <c r="G7" s="55">
+        <v>23</v>
+      </c>
+      <c r="H7" s="54" t="s">
+        <v>135</v>
+      </c>
+      <c r="I7" s="56">
+        <v>39</v>
+      </c>
+      <c r="J7" s="37">
+        <v>10101</v>
+      </c>
+      <c r="K7" s="56" t="s">
+        <v>223</v>
+      </c>
+      <c r="L7" s="37">
+        <v>400</v>
+      </c>
+      <c r="M7" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="N7" s="58"/>
+      <c r="O7" s="58"/>
+      <c r="P7" s="58"/>
+      <c r="Q7" s="58"/>
+      <c r="R7" s="58"/>
+      <c r="S7" s="58"/>
+      <c r="T7" s="58"/>
+      <c r="U7" s="58"/>
+      <c r="V7" s="58"/>
+      <c r="W7" s="58"/>
+      <c r="X7" s="58"/>
+      <c r="Y7" s="58"/>
+      <c r="Z7" s="58"/>
+      <c r="AA7" s="58"/>
+      <c r="AB7" s="58"/>
+      <c r="AC7" s="58"/>
+      <c r="AD7" s="58"/>
+    </row>
+    <row r="8" spans="1:30" s="59" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A8" s="54" t="s">
+        <v>228</v>
+      </c>
+      <c r="B8" s="54" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="55" t="s">
+        <v>229</v>
+      </c>
+      <c r="F8" s="55" t="s">
+        <v>222</v>
+      </c>
+      <c r="G8" s="55">
+        <v>23</v>
+      </c>
+      <c r="H8" s="54" t="s">
+        <v>135</v>
+      </c>
+      <c r="I8" s="56">
+        <v>39</v>
+      </c>
+      <c r="J8" s="37">
+        <v>10101</v>
+      </c>
+      <c r="K8" s="56" t="s">
+        <v>223</v>
+      </c>
+      <c r="L8" s="37">
+        <v>400</v>
+      </c>
+      <c r="M8" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="N8" s="58"/>
+      <c r="O8" s="58"/>
+      <c r="P8" s="58"/>
+      <c r="Q8" s="58"/>
+      <c r="R8" s="58"/>
+      <c r="S8" s="58"/>
+      <c r="T8" s="58"/>
+      <c r="U8" s="58"/>
+      <c r="V8" s="58"/>
+      <c r="W8" s="58"/>
+      <c r="X8" s="58"/>
+      <c r="Y8" s="58"/>
+      <c r="Z8" s="58"/>
+      <c r="AA8" s="58"/>
+      <c r="AB8" s="58"/>
+      <c r="AC8" s="58"/>
+      <c r="AD8" s="58"/>
+    </row>
+    <row r="9" spans="1:30" s="59" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A9" s="54" t="s">
+        <v>230</v>
+      </c>
+      <c r="B9" s="54" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="55" t="s">
+        <v>229</v>
+      </c>
+      <c r="F9" s="55" t="s">
+        <v>222</v>
+      </c>
+      <c r="G9" s="55">
+        <v>-23</v>
+      </c>
+      <c r="H9" s="54" t="s">
+        <v>135</v>
+      </c>
+      <c r="I9" s="56">
+        <v>39</v>
+      </c>
+      <c r="J9" s="37">
+        <v>10101</v>
+      </c>
+      <c r="K9" s="56" t="s">
+        <v>223</v>
+      </c>
+      <c r="L9" s="37">
+        <v>400</v>
+      </c>
+      <c r="M9" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="N9" s="58"/>
+      <c r="O9" s="58"/>
+      <c r="P9" s="58"/>
+      <c r="Q9" s="58"/>
+      <c r="R9" s="58"/>
+      <c r="S9" s="58"/>
+      <c r="T9" s="58"/>
+      <c r="U9" s="58"/>
+      <c r="V9" s="58"/>
+      <c r="W9" s="58"/>
+      <c r="X9" s="58"/>
+      <c r="Y9" s="58"/>
+      <c r="Z9" s="58"/>
+      <c r="AA9" s="58"/>
+      <c r="AB9" s="58"/>
+      <c r="AC9" s="58"/>
+      <c r="AD9" s="58"/>
+    </row>
+    <row r="10" spans="1:30" s="59" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A10" s="54" t="s">
+        <v>140</v>
+      </c>
+      <c r="B10" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="C10" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="55" t="s">
+        <v>221</v>
+      </c>
+      <c r="F10" s="55" t="s">
+        <v>222</v>
+      </c>
+      <c r="G10" s="55">
+        <v>67</v>
+      </c>
+      <c r="H10" s="54" t="s">
+        <v>135</v>
+      </c>
+      <c r="I10" s="56">
+        <v>39</v>
+      </c>
+      <c r="J10" s="37">
+        <v>10101</v>
+      </c>
+      <c r="K10" s="56" t="s">
+        <v>223</v>
+      </c>
+      <c r="L10" s="37">
         <v>404</v>
       </c>
-      <c r="K6" s="36" t="s">
+      <c r="M10" s="54" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="7" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A7" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="B7" s="36" t="s">
-        <v>134</v>
-      </c>
-      <c r="C7" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="37" t="s">
-        <v>135</v>
-      </c>
-      <c r="F7" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="G7" s="37">
-        <v>16331</v>
-      </c>
-      <c r="H7" s="36" t="s">
-        <v>144</v>
-      </c>
-      <c r="I7" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="J7" s="37">
-        <v>400</v>
-      </c>
-      <c r="K7" s="36" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A8" s="36" t="s">
-        <v>145</v>
-      </c>
-      <c r="B8" s="36" t="s">
-        <v>134</v>
-      </c>
-      <c r="C8" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="37" t="s">
-        <v>135</v>
-      </c>
-      <c r="F8" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="G8" s="37">
-        <v>16335</v>
-      </c>
-      <c r="H8" s="37">
-        <v>10101</v>
-      </c>
-      <c r="I8" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="J8" s="37">
-        <v>400</v>
-      </c>
-      <c r="K8" s="36" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A9" s="36" t="s">
-        <v>146</v>
-      </c>
-      <c r="B9" s="36" t="s">
-        <v>134</v>
-      </c>
-      <c r="C9" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="37" t="s">
-        <v>135</v>
-      </c>
-      <c r="F9" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="G9" s="37">
-        <v>16331</v>
-      </c>
-      <c r="H9" s="37">
-        <v>10101</v>
-      </c>
-      <c r="I9" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="J9" s="37">
-        <v>201</v>
-      </c>
-      <c r="K9" s="36" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A10" s="33" t="s">
-        <v>160</v>
-      </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="35"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="11"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="11"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="11"/>
-      <c r="U10" s="11"/>
-      <c r="V10" s="11"/>
-      <c r="W10" s="11"/>
-      <c r="X10" s="11"/>
-      <c r="Y10" s="11"/>
-      <c r="Z10" s="11"/>
-      <c r="AA10" s="11"/>
-      <c r="AB10" s="11"/>
-    </row>
-    <row r="11" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A11" s="36" t="s">
-        <v>147</v>
-      </c>
-      <c r="B11" s="36" t="s">
-        <v>134</v>
+      <c r="N10" s="58"/>
+      <c r="O10" s="58"/>
+      <c r="P10" s="58"/>
+      <c r="Q10" s="58"/>
+      <c r="R10" s="58"/>
+      <c r="S10" s="58"/>
+      <c r="T10" s="58"/>
+      <c r="U10" s="58"/>
+      <c r="V10" s="58"/>
+      <c r="W10" s="58"/>
+      <c r="X10" s="58"/>
+      <c r="Y10" s="58"/>
+      <c r="Z10" s="58"/>
+      <c r="AA10" s="58"/>
+      <c r="AB10" s="58"/>
+      <c r="AC10" s="58"/>
+      <c r="AD10" s="58"/>
+    </row>
+    <row r="11" spans="1:30" s="59" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A11" s="54" t="s">
+        <v>231</v>
+      </c>
+      <c r="B11" s="54" t="s">
+        <v>133</v>
       </c>
       <c r="C11" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="37" t="s">
+      <c r="D11" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="55" t="s">
+        <v>229</v>
+      </c>
+      <c r="F11" s="55" t="s">
+        <v>222</v>
+      </c>
+      <c r="G11" s="55">
+        <v>23</v>
+      </c>
+      <c r="H11" s="54" t="s">
+        <v>232</v>
+      </c>
+      <c r="I11" s="56">
+        <v>39</v>
+      </c>
+      <c r="J11" s="37">
+        <v>10101</v>
+      </c>
+      <c r="K11" s="56" t="s">
+        <v>223</v>
+      </c>
+      <c r="L11" s="37">
+        <v>400</v>
+      </c>
+      <c r="M11" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="N11" s="58"/>
+      <c r="O11" s="58"/>
+      <c r="P11" s="58"/>
+      <c r="Q11" s="58"/>
+      <c r="R11" s="58"/>
+      <c r="S11" s="58"/>
+      <c r="T11" s="58"/>
+      <c r="U11" s="58"/>
+      <c r="V11" s="58"/>
+      <c r="W11" s="58"/>
+      <c r="X11" s="58"/>
+      <c r="Y11" s="58"/>
+      <c r="Z11" s="58"/>
+      <c r="AA11" s="58"/>
+      <c r="AB11" s="58"/>
+      <c r="AC11" s="58"/>
+      <c r="AD11" s="58"/>
+    </row>
+    <row r="12" spans="1:30" s="59" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A12" s="54" t="s">
+        <v>142</v>
+      </c>
+      <c r="B12" s="54" t="s">
+        <v>133</v>
+      </c>
+      <c r="C12" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="55" t="s">
+        <v>221</v>
+      </c>
+      <c r="F12" s="55" t="s">
+        <v>222</v>
+      </c>
+      <c r="G12" s="55">
+        <v>89</v>
+      </c>
+      <c r="H12" s="54" t="s">
         <v>135</v>
       </c>
-      <c r="F11" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="G11" s="37">
-        <v>16331</v>
-      </c>
-      <c r="H11" s="37">
-        <v>18000</v>
-      </c>
-      <c r="I11" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="J11" s="37">
-        <v>404</v>
-      </c>
-      <c r="K11" s="36" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A12" s="36" t="s">
-        <v>148</v>
-      </c>
-      <c r="B12" s="36" t="s">
-        <v>134</v>
-      </c>
-      <c r="C12" s="36" t="s">
+      <c r="I12" s="56">
+        <v>39</v>
+      </c>
+      <c r="J12" s="54" t="s">
+        <v>143</v>
+      </c>
+      <c r="K12" s="56" t="s">
+        <v>223</v>
+      </c>
+      <c r="L12" s="37">
+        <v>400</v>
+      </c>
+      <c r="M12" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="N12" s="58"/>
+      <c r="O12" s="58"/>
+      <c r="P12" s="58"/>
+      <c r="Q12" s="58"/>
+      <c r="R12" s="58"/>
+      <c r="S12" s="58"/>
+      <c r="T12" s="58"/>
+      <c r="U12" s="58"/>
+      <c r="V12" s="58"/>
+      <c r="W12" s="58"/>
+      <c r="X12" s="58"/>
+      <c r="Y12" s="58"/>
+      <c r="Z12" s="58"/>
+      <c r="AA12" s="58"/>
+      <c r="AB12" s="58"/>
+      <c r="AC12" s="58"/>
+      <c r="AD12" s="58"/>
+    </row>
+    <row r="13" spans="1:30" s="59" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A13" s="54" t="s">
+        <v>144</v>
+      </c>
+      <c r="B13" s="54" t="s">
+        <v>133</v>
+      </c>
+      <c r="C13" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="37" t="s">
+      <c r="D13" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="55" t="s">
+        <v>221</v>
+      </c>
+      <c r="F13" s="55" t="s">
+        <v>222</v>
+      </c>
+      <c r="G13" s="55">
+        <v>34</v>
+      </c>
+      <c r="H13" s="54" t="s">
         <v>135</v>
       </c>
-      <c r="F12" s="36"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37">
+      <c r="I13" s="56">
+        <v>73</v>
+      </c>
+      <c r="J13" s="37">
         <v>10101</v>
       </c>
-      <c r="I12" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="J12" s="37">
+      <c r="K13" s="56" t="s">
+        <v>223</v>
+      </c>
+      <c r="L13" s="37">
         <v>400</v>
       </c>
-      <c r="K12" s="36" t="s">
+      <c r="M13" s="54" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="13" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A13" s="36" t="s">
-        <v>149</v>
-      </c>
-      <c r="B13" s="36" t="s">
-        <v>134</v>
-      </c>
-      <c r="C13" s="36" t="s">
+      <c r="N13" s="58"/>
+      <c r="O13" s="58"/>
+      <c r="P13" s="58"/>
+      <c r="Q13" s="58"/>
+      <c r="R13" s="58"/>
+      <c r="S13" s="58"/>
+      <c r="T13" s="58"/>
+      <c r="U13" s="58"/>
+      <c r="V13" s="58"/>
+      <c r="W13" s="58"/>
+      <c r="X13" s="58"/>
+      <c r="Y13" s="58"/>
+      <c r="Z13" s="58"/>
+      <c r="AA13" s="58"/>
+      <c r="AB13" s="58"/>
+      <c r="AC13" s="58"/>
+      <c r="AD13" s="58"/>
+    </row>
+    <row r="14" spans="1:30" s="59" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A14" s="56" t="s">
+        <v>145</v>
+      </c>
+      <c r="B14" s="56" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13" s="37" t="s">
+      <c r="D14" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="55" t="s">
+        <v>233</v>
+      </c>
+      <c r="F14" s="55" t="s">
+        <v>222</v>
+      </c>
+      <c r="G14" s="55">
+        <v>44</v>
+      </c>
+      <c r="H14" s="56" t="s">
         <v>135</v>
       </c>
-      <c r="F13" s="36" t="s">
-        <v>150</v>
-      </c>
-      <c r="G13" s="37">
-        <v>16331</v>
-      </c>
-      <c r="H13" s="37">
+      <c r="I14" s="56">
+        <v>39</v>
+      </c>
+      <c r="J14" s="56">
         <v>10101</v>
       </c>
-      <c r="I13" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="J13" s="37">
-        <v>400</v>
-      </c>
-      <c r="K13" s="36" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A14" s="36" t="s">
-        <v>151</v>
-      </c>
-      <c r="B14" s="36" t="s">
-        <v>142</v>
-      </c>
-      <c r="C14" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="37" t="s">
-        <v>135</v>
-      </c>
-      <c r="F14" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="G14" s="37">
-        <v>16331</v>
-      </c>
-      <c r="H14" s="37">
-        <v>18000</v>
-      </c>
-      <c r="I14" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="J14" s="37">
-        <v>404</v>
-      </c>
-      <c r="K14" s="36" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="15" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A15" s="36" t="s">
-        <v>152</v>
-      </c>
-      <c r="B15" s="36" t="s">
-        <v>134</v>
-      </c>
-      <c r="C15" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="37" t="s">
-        <v>135</v>
-      </c>
-      <c r="F15" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="G15" s="37">
-        <v>16407</v>
-      </c>
-      <c r="H15" s="37">
-        <v>10101</v>
-      </c>
-      <c r="I15" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="J15" s="37">
-        <v>400</v>
-      </c>
-      <c r="K15" s="36" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:28" ht="14.25" customHeight="1">
+      <c r="K14" s="56" t="s">
+        <v>223</v>
+      </c>
+      <c r="L14" s="56">
+        <v>201</v>
+      </c>
+      <c r="M14" s="56" t="s">
+        <v>139</v>
+      </c>
+      <c r="N14" s="58"/>
+      <c r="O14" s="58"/>
+      <c r="P14" s="58"/>
+      <c r="Q14" s="58"/>
+      <c r="R14" s="58"/>
+      <c r="S14" s="58"/>
+      <c r="T14" s="58"/>
+      <c r="U14" s="58"/>
+      <c r="V14" s="58"/>
+      <c r="W14" s="58"/>
+      <c r="X14" s="58"/>
+      <c r="Y14" s="58"/>
+      <c r="Z14" s="58"/>
+      <c r="AA14" s="58"/>
+      <c r="AB14" s="58"/>
+      <c r="AC14" s="58"/>
+      <c r="AD14" s="58"/>
+    </row>
+    <row r="15" spans="1:30" ht="14.25" customHeight="1">
+      <c r="A15" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="34"/>
+      <c r="M15" s="35"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="11"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="11"/>
+      <c r="X15" s="11"/>
+      <c r="Y15" s="11"/>
+      <c r="Z15" s="11"/>
+      <c r="AA15" s="11"/>
+      <c r="AB15" s="11"/>
+      <c r="AC15" s="11"/>
+      <c r="AD15" s="11"/>
+    </row>
+    <row r="16" spans="1:30" ht="14.25" customHeight="1">
       <c r="A16" s="36" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B16" s="36" t="s">
-        <v>134</v>
-      </c>
-      <c r="C16" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="C16" s="37" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="36" t="s">
         <v>56</v>
       </c>
       <c r="E16" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="F16" s="36" t="s">
+      <c r="I16" s="37">
+        <v>16331</v>
+      </c>
+      <c r="J16" s="37">
+        <v>18000</v>
+      </c>
+      <c r="K16" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="G16" s="37">
-        <v>16331</v>
-      </c>
-      <c r="H16" s="37">
-        <v>8658</v>
-      </c>
-      <c r="I16" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="J16" s="37">
-        <v>200</v>
-      </c>
-      <c r="K16" s="36" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="17" spans="1:28" ht="14.25" customHeight="1">
+      <c r="L16" s="37">
+        <v>404</v>
+      </c>
+      <c r="M16" s="36" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" ht="14.25" customHeight="1">
       <c r="A17" s="36" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B17" s="36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C17" s="36" t="s">
         <v>10</v>
@@ -32747,593 +33093,681 @@
         <v>56</v>
       </c>
       <c r="E17" s="37" t="s">
-        <v>135</v>
-      </c>
-      <c r="F17" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37">
+        <v>10101</v>
+      </c>
+      <c r="K17" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="G17" s="37">
+      <c r="L17" s="37">
+        <v>400</v>
+      </c>
+      <c r="M17" s="36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" ht="14.25" customHeight="1">
+      <c r="A18" s="36" t="s">
+        <v>148</v>
+      </c>
+      <c r="B18" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="I18" s="37">
         <v>16331</v>
       </c>
-      <c r="H17" s="37">
+      <c r="J18" s="37">
         <v>10101</v>
       </c>
-      <c r="I17" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="J17" s="37">
-        <v>200</v>
-      </c>
-      <c r="K17" s="36" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A18" s="33" t="s">
-        <v>161</v>
-      </c>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
-      <c r="N18" s="11"/>
-      <c r="O18" s="11"/>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="11"/>
-      <c r="R18" s="11"/>
-      <c r="S18" s="11"/>
-      <c r="T18" s="11"/>
-      <c r="U18" s="11"/>
-      <c r="V18" s="11"/>
-      <c r="W18" s="11"/>
-      <c r="X18" s="11"/>
-      <c r="Y18" s="11"/>
-      <c r="Z18" s="11"/>
-      <c r="AA18" s="11"/>
-      <c r="AB18" s="11"/>
-    </row>
-    <row r="19" spans="1:28" ht="14.25" customHeight="1">
+      <c r="K18" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="L18" s="37">
+        <v>400</v>
+      </c>
+      <c r="M18" s="36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" ht="14.25" customHeight="1">
       <c r="A19" s="36" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="C19" s="36" t="s">
         <v>10</v>
       </c>
       <c r="D19" s="36" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="E19" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="F19" s="36" t="s">
+      <c r="I19" s="37">
+        <v>16331</v>
+      </c>
+      <c r="J19" s="37">
+        <v>18000</v>
+      </c>
+      <c r="K19" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="G19" s="37">
-        <v>16335</v>
-      </c>
-      <c r="H19" s="37">
-        <v>10101</v>
-      </c>
-      <c r="I19" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="J19" s="37">
+      <c r="L19" s="37">
         <v>404</v>
       </c>
-      <c r="K19" s="36" t="s">
+      <c r="M19" s="36" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A20" s="37" t="s">
-        <v>155</v>
+    <row r="20" spans="1:30" ht="14.25" customHeight="1">
+      <c r="A20" s="36" t="s">
+        <v>151</v>
       </c>
       <c r="B20" s="36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C20" s="36" t="s">
         <v>10</v>
       </c>
       <c r="D20" s="36" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="E20" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="F20" s="36" t="s">
+      <c r="I20" s="37">
+        <v>16407</v>
+      </c>
+      <c r="J20" s="37">
+        <v>10101</v>
+      </c>
+      <c r="K20" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="G20" s="37">
-        <v>16335</v>
-      </c>
-      <c r="H20" s="37">
-        <v>10101</v>
-      </c>
-      <c r="I20" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="J20" s="37">
-        <v>404</v>
-      </c>
-      <c r="K20" s="36" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="21" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A21" s="37" t="s">
-        <v>156</v>
+      <c r="L20" s="37">
+        <v>400</v>
+      </c>
+      <c r="M20" s="36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" ht="14.25" customHeight="1">
+      <c r="A21" s="36" t="s">
+        <v>152</v>
       </c>
       <c r="B21" s="36" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="C21" s="36" t="s">
         <v>10</v>
       </c>
       <c r="D21" s="36" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="E21" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="F21" s="36" t="s">
+      <c r="I21" s="37">
+        <v>16331</v>
+      </c>
+      <c r="J21" s="37">
+        <v>8658</v>
+      </c>
+      <c r="K21" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="G21" s="37">
-        <v>16331</v>
-      </c>
-      <c r="H21" s="37">
-        <v>10101</v>
-      </c>
-      <c r="I21" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="J21" s="37">
-        <v>404</v>
-      </c>
-      <c r="K21" s="36" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="22" spans="1:28" ht="14.25" customHeight="1">
+      <c r="L21" s="37">
+        <v>200</v>
+      </c>
+      <c r="M21" s="36" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" ht="14.25" customHeight="1">
       <c r="A22" s="36" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C22" s="36" t="s">
         <v>10</v>
       </c>
       <c r="D22" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="I22" s="37">
+        <v>16331</v>
+      </c>
+      <c r="J22" s="37">
+        <v>10101</v>
+      </c>
+      <c r="K22" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="L22" s="37">
+        <v>200</v>
+      </c>
+      <c r="M22" s="36" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" ht="14.25" customHeight="1">
+      <c r="A23" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="34"/>
+      <c r="L23" s="34"/>
+      <c r="M23" s="35"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
+      <c r="S23" s="11"/>
+      <c r="T23" s="11"/>
+      <c r="U23" s="11"/>
+      <c r="V23" s="11"/>
+      <c r="W23" s="11"/>
+      <c r="X23" s="11"/>
+      <c r="Y23" s="11"/>
+      <c r="Z23" s="11"/>
+      <c r="AA23" s="11"/>
+      <c r="AB23" s="11"/>
+      <c r="AC23" s="11"/>
+      <c r="AD23" s="11"/>
+    </row>
+    <row r="24" spans="1:30" ht="14.25" customHeight="1">
+      <c r="A24" s="36" t="s">
+        <v>161</v>
+      </c>
+      <c r="B24" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="C24" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="37" t="s">
+      <c r="E24" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="F22" s="36" t="s">
+      <c r="I24" s="37">
+        <v>16335</v>
+      </c>
+      <c r="J24" s="37">
+        <v>10101</v>
+      </c>
+      <c r="K24" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="G22" s="37">
-        <v>16331</v>
-      </c>
-      <c r="H22" s="37">
-        <v>10101</v>
-      </c>
-      <c r="I22" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="J22" s="37">
+      <c r="L24" s="37">
         <v>404</v>
       </c>
-      <c r="K22" s="36" t="s">
+      <c r="M24" s="36" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A23" s="37" t="s">
-        <v>158</v>
-      </c>
-      <c r="B23" s="36" t="s">
+    <row r="25" spans="1:30" ht="14.25" customHeight="1">
+      <c r="A25" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="B25" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="C25" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="37" t="s">
         <v>134</v>
-      </c>
-      <c r="C23" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="E23" s="37" t="s">
-        <v>135</v>
-      </c>
-      <c r="F23" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="G23" s="37">
-        <v>16331</v>
-      </c>
-      <c r="H23" s="37">
-        <v>10101</v>
-      </c>
-      <c r="I23" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="J23" s="37">
-        <v>200</v>
-      </c>
-      <c r="K23" s="36" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="24" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A24" s="38" t="s">
-        <v>173</v>
-      </c>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="35"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
-      <c r="N24" s="11"/>
-      <c r="O24" s="11"/>
-      <c r="P24" s="11"/>
-      <c r="Q24" s="11"/>
-      <c r="R24" s="11"/>
-      <c r="S24" s="11"/>
-      <c r="T24" s="11"/>
-      <c r="U24" s="11"/>
-      <c r="V24" s="11"/>
-      <c r="W24" s="11"/>
-      <c r="X24" s="11"/>
-      <c r="Y24" s="11"/>
-      <c r="Z24" s="11"/>
-      <c r="AA24" s="11"/>
-      <c r="AB24" s="11"/>
-    </row>
-    <row r="25" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A25" s="39" t="s">
-        <v>163</v>
-      </c>
-      <c r="B25" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="C25" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="41" t="s">
-        <v>111</v>
-      </c>
-      <c r="E25" s="37" t="s">
-        <v>135</v>
       </c>
       <c r="F25" s="37"/>
       <c r="G25" s="37"/>
-      <c r="H25" s="37">
+      <c r="H25" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="I25" s="37">
+        <v>16335</v>
+      </c>
+      <c r="J25" s="37">
         <v>10101</v>
       </c>
-      <c r="I25" s="37"/>
-      <c r="J25" s="42">
-        <v>200</v>
-      </c>
-      <c r="K25" s="40" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="26" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A26" s="40" t="s">
-        <v>166</v>
-      </c>
-      <c r="B26" s="43" t="s">
-        <v>167</v>
-      </c>
-      <c r="C26" s="40" t="s">
+      <c r="K25" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="L25" s="37">
+        <v>404</v>
+      </c>
+      <c r="M25" s="36" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" ht="14.25" customHeight="1">
+      <c r="A26" s="37" t="s">
+        <v>155</v>
+      </c>
+      <c r="B26" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="C26" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="41" t="s">
-        <v>111</v>
+      <c r="D26" s="36" t="s">
+        <v>21</v>
       </c>
       <c r="E26" s="37" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F26" s="37"/>
       <c r="G26" s="37"/>
-      <c r="H26" s="37">
+      <c r="H26" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="I26" s="37">
+        <v>16331</v>
+      </c>
+      <c r="J26" s="37">
         <v>10101</v>
       </c>
-      <c r="I26" s="37"/>
-      <c r="J26" s="42">
+      <c r="K26" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="L26" s="37">
         <v>404</v>
       </c>
-      <c r="K26" s="40" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A27" s="40" t="s">
-        <v>169</v>
-      </c>
-      <c r="B27" s="43" t="s">
+      <c r="M26" s="36" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" ht="14.25" customHeight="1">
+      <c r="A27" s="36" t="s">
+        <v>156</v>
+      </c>
+      <c r="B27" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="C27" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="37" t="s">
         <v>134</v>
-      </c>
-      <c r="C27" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="41" t="s">
-        <v>111</v>
-      </c>
-      <c r="E27" s="37" t="s">
-        <v>135</v>
       </c>
       <c r="F27" s="37"/>
       <c r="G27" s="37"/>
-      <c r="H27" s="37">
+      <c r="H27" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="I27" s="37">
+        <v>16331</v>
+      </c>
+      <c r="J27" s="37">
         <v>10101</v>
       </c>
-      <c r="I27" s="37"/>
-      <c r="J27" s="42">
+      <c r="K27" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="L27" s="37">
         <v>404</v>
       </c>
-      <c r="K27" s="40" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="28" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A28" s="39" t="s">
-        <v>170</v>
-      </c>
-      <c r="B28" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="C28" s="40" t="s">
+      <c r="M27" s="36" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" ht="14.25" customHeight="1">
+      <c r="A28" s="37" t="s">
+        <v>157</v>
+      </c>
+      <c r="B28" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="C28" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D28" s="41" t="s">
-        <v>11</v>
+      <c r="D28" s="36" t="s">
+        <v>21</v>
       </c>
       <c r="E28" s="37" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F28" s="37"/>
       <c r="G28" s="37"/>
-      <c r="H28" s="37">
+      <c r="H28" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="I28" s="37">
+        <v>16331</v>
+      </c>
+      <c r="J28" s="37">
         <v>10101</v>
       </c>
-      <c r="I28" s="37"/>
-      <c r="J28" s="42">
-        <v>405</v>
-      </c>
-      <c r="K28" s="44" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="29" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A29" s="39" t="s">
+      <c r="K28" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="L28" s="37">
+        <v>200</v>
+      </c>
+      <c r="M28" s="36" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" ht="14.25" customHeight="1">
+      <c r="A29" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="B29" s="40" t="s">
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="34"/>
+      <c r="J29" s="34"/>
+      <c r="K29" s="34"/>
+      <c r="L29" s="34"/>
+      <c r="M29" s="35"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="11"/>
+      <c r="R29" s="11"/>
+      <c r="S29" s="11"/>
+      <c r="T29" s="11"/>
+      <c r="U29" s="11"/>
+      <c r="V29" s="11"/>
+      <c r="W29" s="11"/>
+      <c r="X29" s="11"/>
+      <c r="Y29" s="11"/>
+      <c r="Z29" s="11"/>
+      <c r="AA29" s="11"/>
+      <c r="AB29" s="11"/>
+      <c r="AC29" s="11"/>
+      <c r="AD29" s="11"/>
+    </row>
+    <row r="30" spans="1:30" ht="14.25" customHeight="1">
+      <c r="A30" s="39" t="s">
+        <v>162</v>
+      </c>
+      <c r="B30" s="40" t="s">
+        <v>163</v>
+      </c>
+      <c r="C30" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="E30" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="37"/>
+      <c r="J30" s="37">
+        <v>10101</v>
+      </c>
+      <c r="K30" s="37"/>
+      <c r="L30" s="42">
+        <v>200</v>
+      </c>
+      <c r="M30" s="40" t="s">
         <v>164</v>
       </c>
-      <c r="C29" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="41" t="s">
-        <v>111</v>
-      </c>
-      <c r="E29" s="37" t="s">
-        <v>135</v>
-      </c>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37">
-        <v>10101</v>
-      </c>
-      <c r="I29" s="37"/>
-      <c r="J29" s="42">
-        <v>401</v>
-      </c>
-      <c r="K29" s="40" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A30" s="45" t="s">
-        <v>174</v>
-      </c>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="34"/>
-      <c r="H30" s="34"/>
-      <c r="I30" s="34"/>
-      <c r="J30" s="34"/>
-      <c r="K30" s="35"/>
-      <c r="L30" s="11"/>
-      <c r="M30" s="11"/>
-      <c r="N30" s="11"/>
-      <c r="O30" s="11"/>
-      <c r="P30" s="11"/>
-      <c r="Q30" s="11"/>
-      <c r="R30" s="11"/>
-      <c r="S30" s="11"/>
-      <c r="T30" s="11"/>
-      <c r="U30" s="11"/>
-      <c r="V30" s="11"/>
-      <c r="W30" s="11"/>
-      <c r="X30" s="11"/>
-      <c r="Y30" s="11"/>
-      <c r="Z30" s="11"/>
-      <c r="AA30" s="11"/>
-      <c r="AB30" s="11"/>
-    </row>
-    <row r="31" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A31" t="s">
-        <v>176</v>
-      </c>
-      <c r="B31" s="40" t="s">
-        <v>164</v>
+    </row>
+    <row r="31" spans="1:30" ht="14.25" customHeight="1">
+      <c r="A31" s="40" t="s">
+        <v>165</v>
+      </c>
+      <c r="B31" s="43" t="s">
+        <v>166</v>
       </c>
       <c r="C31" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="D31" s="36" t="s">
-        <v>21</v>
+      <c r="D31" s="41" t="s">
+        <v>111</v>
       </c>
       <c r="E31" s="37" t="s">
-        <v>135</v>
-      </c>
-      <c r="J31" s="42">
-        <v>200</v>
-      </c>
-      <c r="K31" s="40" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="32" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A32" t="s">
-        <v>177</v>
-      </c>
-      <c r="B32" s="40" t="s">
-        <v>164</v>
+        <v>134</v>
+      </c>
+      <c r="F31" s="37"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="37"/>
+      <c r="J31" s="37">
+        <v>10101</v>
+      </c>
+      <c r="K31" s="37"/>
+      <c r="L31" s="42">
+        <v>404</v>
+      </c>
+      <c r="M31" s="40" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" ht="14.25" customHeight="1">
+      <c r="A32" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="B32" s="43" t="s">
+        <v>133</v>
       </c>
       <c r="C32" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="D32" s="36" t="s">
-        <v>21</v>
+      <c r="D32" s="41" t="s">
+        <v>111</v>
       </c>
       <c r="E32" s="37" t="s">
-        <v>135</v>
-      </c>
-      <c r="J32" s="42">
+        <v>134</v>
+      </c>
+      <c r="F32" s="37"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
+      <c r="I32" s="37"/>
+      <c r="J32" s="37">
+        <v>10101</v>
+      </c>
+      <c r="K32" s="37"/>
+      <c r="L32" s="42">
         <v>404</v>
       </c>
-      <c r="K32" s="40" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="33" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A33" t="s">
-        <v>178</v>
+      <c r="M32" s="40" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="33" spans="1:30" ht="14.25" customHeight="1">
+      <c r="A33" s="39" t="s">
+        <v>169</v>
       </c>
       <c r="B33" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C33" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="D33" s="36" t="s">
-        <v>21</v>
+      <c r="D33" s="41" t="s">
+        <v>11</v>
       </c>
       <c r="E33" s="37" t="s">
-        <v>135</v>
-      </c>
-      <c r="J33" s="42">
-        <v>404</v>
-      </c>
-      <c r="K33" s="40" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="34" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A34" t="s">
-        <v>179</v>
+        <v>134</v>
+      </c>
+      <c r="F33" s="37"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="37"/>
+      <c r="I33" s="37"/>
+      <c r="J33" s="37">
+        <v>10101</v>
+      </c>
+      <c r="K33" s="37"/>
+      <c r="L33" s="42">
+        <v>405</v>
+      </c>
+      <c r="M33" s="44" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="34" spans="1:30" ht="14.25" customHeight="1">
+      <c r="A34" s="39" t="s">
+        <v>171</v>
       </c>
       <c r="B34" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C34" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="D34" s="36" t="s">
+      <c r="D34" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="E34" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="F34" s="37"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="37"/>
+      <c r="I34" s="37"/>
+      <c r="J34" s="37">
+        <v>10101</v>
+      </c>
+      <c r="K34" s="37"/>
+      <c r="L34" s="42">
+        <v>401</v>
+      </c>
+      <c r="M34" s="40" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:30" ht="14.25" customHeight="1">
+      <c r="A35" s="45" t="s">
+        <v>173</v>
+      </c>
+      <c r="B35" s="34"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="34"/>
+      <c r="H35" s="34"/>
+      <c r="I35" s="34"/>
+      <c r="J35" s="34"/>
+      <c r="K35" s="34"/>
+      <c r="L35" s="34"/>
+      <c r="M35" s="35"/>
+      <c r="N35" s="11"/>
+      <c r="O35" s="11"/>
+      <c r="P35" s="11"/>
+      <c r="Q35" s="11"/>
+      <c r="R35" s="11"/>
+      <c r="S35" s="11"/>
+      <c r="T35" s="11"/>
+      <c r="U35" s="11"/>
+      <c r="V35" s="11"/>
+      <c r="W35" s="11"/>
+      <c r="X35" s="11"/>
+      <c r="Y35" s="11"/>
+      <c r="Z35" s="11"/>
+      <c r="AA35" s="11"/>
+      <c r="AB35" s="11"/>
+      <c r="AC35" s="11"/>
+      <c r="AD35" s="11"/>
+    </row>
+    <row r="36" spans="1:30" ht="14.25" customHeight="1">
+      <c r="A36" t="s">
+        <v>175</v>
+      </c>
+      <c r="B36" s="40" t="s">
+        <v>163</v>
+      </c>
+      <c r="C36" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="E34" s="37" t="s">
-        <v>135</v>
-      </c>
-      <c r="J34" s="42">
+      <c r="E36" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="L36" s="42">
         <v>200</v>
       </c>
-      <c r="K34" s="40" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="35" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A35" t="s">
-        <v>175</v>
-      </c>
-      <c r="B35" s="40" t="s">
+      <c r="M36" s="40" t="s">
         <v>164</v>
       </c>
-      <c r="C35" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="E35" s="37" t="s">
-        <v>135</v>
-      </c>
-      <c r="J35" s="46">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="36" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A36" s="45" t="s">
-        <v>184</v>
-      </c>
-      <c r="B36" s="34"/>
-      <c r="C36" s="34"/>
-      <c r="D36" s="34"/>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
-      <c r="G36" s="34"/>
-      <c r="H36" s="34"/>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
-      <c r="K36" s="35"/>
-      <c r="L36" s="11"/>
-      <c r="M36" s="11"/>
-      <c r="N36" s="11"/>
-      <c r="O36" s="11"/>
-      <c r="P36" s="11"/>
-      <c r="Q36" s="11"/>
-      <c r="R36" s="11"/>
-      <c r="S36" s="11"/>
-      <c r="T36" s="11"/>
-      <c r="U36" s="11"/>
-      <c r="V36" s="11"/>
-      <c r="W36" s="11"/>
-      <c r="X36" s="11"/>
-      <c r="Y36" s="11"/>
-      <c r="Z36" s="11"/>
-      <c r="AA36" s="11"/>
-      <c r="AB36" s="11"/>
-    </row>
-    <row r="37" spans="1:28" ht="14.25" customHeight="1">
+    </row>
+    <row r="37" spans="1:30" ht="14.25" customHeight="1">
       <c r="A37" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B37" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C37" s="40" t="s">
         <v>10</v>
@@ -33342,24 +33776,21 @@
         <v>21</v>
       </c>
       <c r="E37" s="37" t="s">
-        <v>135</v>
-      </c>
-      <c r="H37" s="37">
-        <v>10101</v>
-      </c>
-      <c r="J37" s="42">
-        <v>200</v>
-      </c>
-      <c r="K37" s="40" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="38" spans="1:28" ht="14.25" customHeight="1">
+        <v>134</v>
+      </c>
+      <c r="L37" s="42">
+        <v>404</v>
+      </c>
+      <c r="M37" s="40" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="38" spans="1:30" ht="14.25" customHeight="1">
       <c r="A38" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B38" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C38" s="40" t="s">
         <v>10</v>
@@ -33368,24 +33799,21 @@
         <v>21</v>
       </c>
       <c r="E38" s="37" t="s">
-        <v>135</v>
-      </c>
-      <c r="H38" s="37">
-        <v>10101</v>
-      </c>
-      <c r="J38" s="42">
-        <v>200</v>
-      </c>
-      <c r="K38" s="40" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="39" spans="1:28" ht="14.25" customHeight="1">
+        <v>134</v>
+      </c>
+      <c r="L38" s="42">
+        <v>404</v>
+      </c>
+      <c r="M38" s="40" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="39" spans="1:30" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B39" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C39" s="40" t="s">
         <v>10</v>
@@ -33394,24 +33822,21 @@
         <v>21</v>
       </c>
       <c r="E39" s="37" t="s">
-        <v>135</v>
-      </c>
-      <c r="H39" s="37">
-        <v>10101</v>
-      </c>
-      <c r="J39" s="42">
-        <v>404</v>
-      </c>
-      <c r="K39" s="40" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="40" spans="1:28" ht="14.25" customHeight="1">
+        <v>134</v>
+      </c>
+      <c r="L39" s="42">
+        <v>200</v>
+      </c>
+      <c r="M39" s="40" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="40" spans="1:30" ht="14.25" customHeight="1">
       <c r="A40" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B40" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C40" s="40" t="s">
         <v>10</v>
@@ -33420,48 +33845,175 @@
         <v>21</v>
       </c>
       <c r="E40" s="37" t="s">
-        <v>135</v>
-      </c>
-      <c r="H40" s="37">
+        <v>134</v>
+      </c>
+      <c r="L40" s="46">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="41" spans="1:30" ht="14.25" customHeight="1">
+      <c r="A41" s="45" t="s">
+        <v>183</v>
+      </c>
+      <c r="B41" s="34"/>
+      <c r="C41" s="34"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="34"/>
+      <c r="G41" s="34"/>
+      <c r="H41" s="34"/>
+      <c r="I41" s="34"/>
+      <c r="J41" s="34"/>
+      <c r="K41" s="34"/>
+      <c r="L41" s="34"/>
+      <c r="M41" s="35"/>
+      <c r="N41" s="11"/>
+      <c r="O41" s="11"/>
+      <c r="P41" s="11"/>
+      <c r="Q41" s="11"/>
+      <c r="R41" s="11"/>
+      <c r="S41" s="11"/>
+      <c r="T41" s="11"/>
+      <c r="U41" s="11"/>
+      <c r="V41" s="11"/>
+      <c r="W41" s="11"/>
+      <c r="X41" s="11"/>
+      <c r="Y41" s="11"/>
+      <c r="Z41" s="11"/>
+      <c r="AA41" s="11"/>
+      <c r="AB41" s="11"/>
+      <c r="AC41" s="11"/>
+      <c r="AD41" s="11"/>
+    </row>
+    <row r="42" spans="1:30" ht="14.25" customHeight="1">
+      <c r="A42" t="s">
+        <v>180</v>
+      </c>
+      <c r="B42" s="40" t="s">
+        <v>163</v>
+      </c>
+      <c r="C42" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="E42" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="J42" s="37">
         <v>10101</v>
       </c>
-      <c r="J40" s="42">
+      <c r="L42" s="42">
+        <v>200</v>
+      </c>
+      <c r="M42" s="40" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="43" spans="1:30" ht="14.25" customHeight="1">
+      <c r="A43" t="s">
+        <v>181</v>
+      </c>
+      <c r="B43" s="40" t="s">
+        <v>163</v>
+      </c>
+      <c r="C43" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="E43" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="J43" s="37">
+        <v>10101</v>
+      </c>
+      <c r="L43" s="42">
+        <v>200</v>
+      </c>
+      <c r="M43" s="40" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="44" spans="1:30" ht="14.25" customHeight="1">
+      <c r="A44" t="s">
+        <v>182</v>
+      </c>
+      <c r="B44" s="40" t="s">
+        <v>163</v>
+      </c>
+      <c r="C44" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="E44" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="J44" s="37">
+        <v>10101</v>
+      </c>
+      <c r="L44" s="42">
         <v>404</v>
       </c>
-      <c r="K40" s="40" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="41" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A41" t="s">
-        <v>180</v>
-      </c>
-      <c r="B41" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="C41" s="40" t="s">
+      <c r="M44" s="40" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="45" spans="1:30" ht="14.25" customHeight="1">
+      <c r="A45" t="s">
+        <v>177</v>
+      </c>
+      <c r="B45" s="40" t="s">
+        <v>163</v>
+      </c>
+      <c r="C45" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="D41" s="36" t="s">
+      <c r="D45" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="E41" s="37" t="s">
-        <v>135</v>
-      </c>
-      <c r="H41" s="37">
+      <c r="E45" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="J45" s="37">
         <v>10101</v>
       </c>
-      <c r="J41" s="46">
+      <c r="L45" s="42">
+        <v>404</v>
+      </c>
+      <c r="M45" s="40" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="46" spans="1:30" ht="14.25" customHeight="1">
+      <c r="A46" t="s">
+        <v>179</v>
+      </c>
+      <c r="B46" s="40" t="s">
+        <v>163</v>
+      </c>
+      <c r="C46" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="E46" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="J46" s="37">
+        <v>10101</v>
+      </c>
+      <c r="L46" s="46">
         <v>401</v>
       </c>
     </row>
-    <row r="42" spans="1:28" ht="14.25" customHeight="1"/>
-    <row r="43" spans="1:28" ht="14.25" customHeight="1"/>
-    <row r="44" spans="1:28" ht="14.25" customHeight="1"/>
-    <row r="45" spans="1:28" ht="14.25" customHeight="1"/>
-    <row r="46" spans="1:28" ht="14.25" customHeight="1"/>
-    <row r="47" spans="1:28" ht="14.25" customHeight="1"/>
-    <row r="48" spans="1:28" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:30" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:30" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -34416,6 +34968,11 @@
     <row r="1000" ht="14.25" customHeight="1"/>
     <row r="1001" ht="14.25" customHeight="1"/>
     <row r="1002" ht="14.25" customHeight="1"/>
+    <row r="1003" ht="14.25" customHeight="1"/>
+    <row r="1004" ht="14.25" customHeight="1"/>
+    <row r="1005" ht="14.25" customHeight="1"/>
+    <row r="1006" ht="14.25" customHeight="1"/>
+    <row r="1007" ht="14.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -34426,8 +34983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4288ABC0-DE51-4F1D-BF0D-EE92A041B4A9}">
   <dimension ref="A1:AF3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -34486,75 +35043,75 @@
         <v>7</v>
       </c>
       <c r="L1" s="49" t="s">
+        <v>186</v>
+      </c>
+      <c r="M1" s="49" t="s">
         <v>187</v>
       </c>
-      <c r="M1" s="49" t="s">
+      <c r="N1" s="49" t="s">
         <v>188</v>
       </c>
-      <c r="N1" s="49" t="s">
+      <c r="O1" s="49" t="s">
         <v>189</v>
       </c>
-      <c r="O1" s="49" t="s">
+      <c r="P1" s="49" t="s">
         <v>190</v>
       </c>
-      <c r="P1" s="49" t="s">
+      <c r="Q1" s="49" t="s">
         <v>191</v>
       </c>
-      <c r="Q1" s="49" t="s">
+      <c r="R1" s="49" t="s">
         <v>192</v>
       </c>
-      <c r="R1" s="49" t="s">
+      <c r="S1" s="49" t="s">
         <v>193</v>
       </c>
-      <c r="S1" s="49" t="s">
+      <c r="T1" s="49" t="s">
         <v>194</v>
       </c>
-      <c r="T1" s="49" t="s">
+      <c r="U1" s="49" t="s">
         <v>195</v>
       </c>
-      <c r="U1" s="49" t="s">
+      <c r="V1" s="49" t="s">
         <v>196</v>
       </c>
-      <c r="V1" s="49" t="s">
+      <c r="W1" s="49" t="s">
         <v>197</v>
       </c>
-      <c r="W1" s="49" t="s">
+      <c r="X1" s="49" t="s">
         <v>198</v>
       </c>
-      <c r="X1" s="49" t="s">
+      <c r="Y1" s="49" t="s">
         <v>199</v>
       </c>
-      <c r="Y1" s="49" t="s">
+      <c r="Z1" s="49" t="s">
         <v>200</v>
       </c>
-      <c r="Z1" s="49" t="s">
+      <c r="AA1" s="49" t="s">
         <v>201</v>
       </c>
-      <c r="AA1" s="49" t="s">
+      <c r="AB1" s="49" t="s">
         <v>202</v>
       </c>
-      <c r="AB1" s="49" t="s">
+      <c r="AC1" s="49" t="s">
         <v>203</v>
       </c>
-      <c r="AC1" s="49" t="s">
+      <c r="AD1" s="49" t="s">
         <v>204</v>
       </c>
-      <c r="AD1" s="49" t="s">
+      <c r="AE1" s="49" t="s">
         <v>205</v>
       </c>
-      <c r="AE1" s="49" t="s">
+      <c r="AF1" s="49" t="s">
         <v>206</v>
-      </c>
-      <c r="AF1" s="49" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:32">
       <c r="A2" s="47" t="s">
+        <v>184</v>
+      </c>
+      <c r="B2" s="48" t="s">
         <v>185</v>
-      </c>
-      <c r="B2" s="48" t="s">
-        <v>186</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -34563,64 +35120,49 @@
         <v>11</v>
       </c>
       <c r="L2" s="50" t="s">
+        <v>207</v>
+      </c>
+      <c r="M2" s="50" t="s">
         <v>208</v>
       </c>
-      <c r="M2" s="50" t="s">
+      <c r="N2" s="50" t="s">
         <v>209</v>
       </c>
-      <c r="N2" s="50" t="s">
+      <c r="O2" s="50" t="s">
+        <v>215</v>
+      </c>
+      <c r="P2" s="50" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q2" s="53" t="s">
+        <v>217</v>
+      </c>
+      <c r="R2" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="O2" s="50" t="s">
-        <v>221</v>
-      </c>
-      <c r="P2" s="50" t="s">
-        <v>222</v>
-      </c>
-      <c r="Q2" s="53" t="s">
-        <v>216</v>
-      </c>
-      <c r="R2" s="50" t="s">
+      <c r="S2" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="S2" s="50" t="s">
+      <c r="T2" s="51" t="s">
+        <v>214</v>
+      </c>
+      <c r="U2" s="52" t="s">
+        <v>218</v>
+      </c>
+      <c r="V2" s="50" t="s">
         <v>212</v>
       </c>
-      <c r="T2" s="51" t="s">
-        <v>215</v>
-      </c>
-      <c r="U2" s="52" t="s">
-        <v>223</v>
-      </c>
-      <c r="V2" s="50" t="s">
+      <c r="W2" s="50" t="s">
         <v>213</v>
-      </c>
-      <c r="W2" s="50" t="s">
-        <v>214</v>
       </c>
       <c r="X2" s="51" t="s">
         <v>219</v>
       </c>
-      <c r="Y2" s="50">
-        <v>11</v>
-      </c>
-      <c r="Z2" s="50" t="s">
-        <v>220</v>
-      </c>
+      <c r="Y2" s="50"/>
+      <c r="Z2" s="50"/>
     </row>
     <row r="3" spans="1:32">
-      <c r="A3" s="47" t="s">
-        <v>217</v>
-      </c>
-      <c r="B3" s="55" t="s">
-        <v>218</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="54" t="s">
-        <v>21</v>
-      </c>
+      <c r="A3" s="47"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>